<commit_message>
Deploying to gh-pages from @ phenopackets/core-ig@fc9d2101d9e2289cdbc3fddcfdc59f742eaa87de 🚀
</commit_message>
<xml_diff>
--- a/StructureDefinition-Biosample.xlsx
+++ b/StructureDefinition-Biosample.xlsx
@@ -9,13 +9,13 @@
     <sheet name="Elements" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AL$59</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AL$57</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1987" uniqueCount="355">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1919" uniqueCount="346">
   <si>
     <t>Path</t>
   </si>
@@ -303,9 +303,6 @@
     <t>Specimen.extension</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
     <t xml:space="preserve">Extension
 </t>
   </si>
@@ -330,44 +327,18 @@
 ext-1:Must have either extensions or value[x], not both {extension.exists() != value.exists()}</t>
   </si>
   <si>
-    <t>PhenotypicFeature</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Extension {https://github.com/phenopackets/core-ig/StructureDefinition/PhenotypicFeatureExt}
+    <t>Taxonomy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extension {https://github.com/phenopackets/core-ig/StructureDefinition/Taxonomy}
 </t>
   </si>
   <si>
-    <t>Phenotypic Feature (Biosample)</t>
-  </si>
-  <si>
-    <t>Term representing phenotypic features of a Biosample</t>
+    <t>Corresponds to taxonomy (GA4GH). For resources where there may be more than one organism being studied it is advisable to indicate the taxonomic identifier of that organism, to its most specific level.</t>
   </si>
   <si>
     <t xml:space="preserve">ele-1
 </t>
-  </si>
-  <si>
-    <t>Measurement</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Extension {https://github.com/phenopackets/core-ig/StructureDefinition/MeasurementExt}
-</t>
-  </si>
-  <si>
-    <t>Measurement (Biosample)</t>
-  </si>
-  <si>
-    <t>Term representing a measurement made on a Biosample</t>
-  </si>
-  <si>
-    <t>Taxonomy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Extension {https://github.com/phenopackets/core-ig/StructureDefinition/Taxonomy}
-</t>
-  </si>
-  <si>
-    <t>Corresponds to taxonomy (GA4GH). For resources where there may be more than one organism being studied it is advisable to indicate the taxonomic identifier of that organism, to its most specific level.</t>
   </si>
   <si>
     <t>HistologicalDiagnosis</t>
@@ -1271,7 +1242,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AL59"/>
+  <dimension ref="A1:AL57"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -2198,7 +2169,7 @@
       </c>
       <c r="D9" s="2"/>
       <c r="E9" t="s" s="2">
-        <v>92</v>
+        <v>40</v>
       </c>
       <c r="F9" t="s" s="2">
         <v>41</v>
@@ -2213,13 +2184,13 @@
         <v>39</v>
       </c>
       <c r="J9" t="s" s="2">
+        <v>92</v>
+      </c>
+      <c r="K9" t="s" s="2">
         <v>93</v>
       </c>
-      <c r="K9" t="s" s="2">
+      <c r="L9" t="s" s="2">
         <v>94</v>
-      </c>
-      <c r="L9" t="s" s="2">
-        <v>95</v>
       </c>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
@@ -2258,17 +2229,17 @@
         <v>39</v>
       </c>
       <c r="AA9" t="s" s="2">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="AB9" s="2"/>
       <c r="AC9" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AD9" t="s" s="2">
+        <v>96</v>
+      </c>
+      <c r="AE9" t="s" s="2">
         <v>97</v>
-      </c>
-      <c r="AE9" t="s" s="2">
-        <v>98</v>
       </c>
       <c r="AF9" t="s" s="2">
         <v>40</v>
@@ -2280,7 +2251,7 @@
         <v>39</v>
       </c>
       <c r="AI9" t="s" s="2">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AJ9" t="s" s="2">
         <v>39</v>
@@ -2297,17 +2268,17 @@
         <v>91</v>
       </c>
       <c r="B10" t="s" s="2">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C10" t="s" s="2">
         <v>39</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="F10" t="s" s="2">
         <v>47</v>
-      </c>
-      <c r="F10" t="s" s="2">
-        <v>41</v>
       </c>
       <c r="G10" t="s" s="2">
         <v>48</v>
@@ -2319,13 +2290,13 @@
         <v>39</v>
       </c>
       <c r="J10" t="s" s="2">
+        <v>100</v>
+      </c>
+      <c r="K10" t="s" s="2">
+        <v>99</v>
+      </c>
+      <c r="L10" t="s" s="2">
         <v>101</v>
-      </c>
-      <c r="K10" t="s" s="2">
-        <v>102</v>
-      </c>
-      <c r="L10" t="s" s="2">
-        <v>103</v>
       </c>
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
@@ -2376,7 +2347,7 @@
         <v>39</v>
       </c>
       <c r="AE10" t="s" s="2">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AF10" t="s" s="2">
         <v>40</v>
@@ -2385,10 +2356,10 @@
         <v>41</v>
       </c>
       <c r="AH10" t="s" s="2">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="AI10" t="s" s="2">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AJ10" t="s" s="2">
         <v>39</v>
@@ -2405,14 +2376,14 @@
         <v>91</v>
       </c>
       <c r="B11" t="s" s="2">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C11" t="s" s="2">
         <v>39</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" t="s" s="2">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="F11" t="s" s="2">
         <v>41</v>
@@ -2427,13 +2398,13 @@
         <v>39</v>
       </c>
       <c r="J11" t="s" s="2">
+        <v>104</v>
+      </c>
+      <c r="K11" t="s" s="2">
+        <v>105</v>
+      </c>
+      <c r="L11" t="s" s="2">
         <v>106</v>
-      </c>
-      <c r="K11" t="s" s="2">
-        <v>107</v>
-      </c>
-      <c r="L11" t="s" s="2">
-        <v>108</v>
       </c>
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
@@ -2484,7 +2455,7 @@
         <v>39</v>
       </c>
       <c r="AE11" t="s" s="2">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AF11" t="s" s="2">
         <v>40</v>
@@ -2493,10 +2464,10 @@
         <v>41</v>
       </c>
       <c r="AH11" t="s" s="2">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="AI11" t="s" s="2">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AJ11" t="s" s="2">
         <v>39</v>
@@ -2513,7 +2484,7 @@
         <v>91</v>
       </c>
       <c r="B12" t="s" s="2">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C12" t="s" s="2">
         <v>39</v>
@@ -2535,13 +2506,13 @@
         <v>39</v>
       </c>
       <c r="J12" t="s" s="2">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="K12" t="s" s="2">
         <v>109</v>
       </c>
       <c r="L12" t="s" s="2">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
@@ -2592,7 +2563,7 @@
         <v>39</v>
       </c>
       <c r="AE12" t="s" s="2">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AF12" t="s" s="2">
         <v>40</v>
@@ -2601,10 +2572,10 @@
         <v>41</v>
       </c>
       <c r="AH12" t="s" s="2">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="AI12" t="s" s="2">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AJ12" t="s" s="2">
         <v>39</v>
@@ -2621,7 +2592,7 @@
         <v>91</v>
       </c>
       <c r="B13" t="s" s="2">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C13" t="s" s="2">
         <v>39</v>
@@ -2643,13 +2614,13 @@
         <v>39</v>
       </c>
       <c r="J13" t="s" s="2">
+        <v>112</v>
+      </c>
+      <c r="K13" t="s" s="2">
         <v>113</v>
       </c>
-      <c r="K13" t="s" s="2">
+      <c r="L13" t="s" s="2">
         <v>114</v>
-      </c>
-      <c r="L13" t="s" s="2">
-        <v>115</v>
       </c>
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
@@ -2700,7 +2671,7 @@
         <v>39</v>
       </c>
       <c r="AE13" t="s" s="2">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AF13" t="s" s="2">
         <v>40</v>
@@ -2709,10 +2680,10 @@
         <v>41</v>
       </c>
       <c r="AH13" t="s" s="2">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="AI13" t="s" s="2">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AJ13" t="s" s="2">
         <v>39</v>
@@ -2729,7 +2700,7 @@
         <v>91</v>
       </c>
       <c r="B14" t="s" s="2">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C14" t="s" s="2">
         <v>39</v>
@@ -2739,7 +2710,7 @@
         <v>40</v>
       </c>
       <c r="F14" t="s" s="2">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="G14" t="s" s="2">
         <v>48</v>
@@ -2751,13 +2722,13 @@
         <v>39</v>
       </c>
       <c r="J14" t="s" s="2">
+        <v>116</v>
+      </c>
+      <c r="K14" t="s" s="2">
         <v>117</v>
       </c>
-      <c r="K14" t="s" s="2">
+      <c r="L14" t="s" s="2">
         <v>118</v>
-      </c>
-      <c r="L14" t="s" s="2">
-        <v>119</v>
       </c>
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
@@ -2808,7 +2779,7 @@
         <v>39</v>
       </c>
       <c r="AE14" t="s" s="2">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AF14" t="s" s="2">
         <v>40</v>
@@ -2817,10 +2788,10 @@
         <v>41</v>
       </c>
       <c r="AH14" t="s" s="2">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="AI14" t="s" s="2">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AJ14" t="s" s="2">
         <v>39</v>
@@ -2837,7 +2808,7 @@
         <v>91</v>
       </c>
       <c r="B15" t="s" s="2">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C15" t="s" s="2">
         <v>39</v>
@@ -2859,13 +2830,13 @@
         <v>39</v>
       </c>
       <c r="J15" t="s" s="2">
+        <v>120</v>
+      </c>
+      <c r="K15" t="s" s="2">
         <v>121</v>
       </c>
-      <c r="K15" t="s" s="2">
+      <c r="L15" t="s" s="2">
         <v>122</v>
-      </c>
-      <c r="L15" t="s" s="2">
-        <v>123</v>
       </c>
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
@@ -2916,7 +2887,7 @@
         <v>39</v>
       </c>
       <c r="AE15" t="s" s="2">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AF15" t="s" s="2">
         <v>40</v>
@@ -2925,10 +2896,10 @@
         <v>41</v>
       </c>
       <c r="AH15" t="s" s="2">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="AI15" t="s" s="2">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AJ15" t="s" s="2">
         <v>39</v>
@@ -2945,7 +2916,7 @@
         <v>91</v>
       </c>
       <c r="B16" t="s" s="2">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C16" t="s" s="2">
         <v>39</v>
@@ -2967,13 +2938,13 @@
         <v>39</v>
       </c>
       <c r="J16" t="s" s="2">
+        <v>124</v>
+      </c>
+      <c r="K16" t="s" s="2">
         <v>125</v>
       </c>
-      <c r="K16" t="s" s="2">
+      <c r="L16" t="s" s="2">
         <v>126</v>
-      </c>
-      <c r="L16" t="s" s="2">
-        <v>127</v>
       </c>
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
@@ -3024,7 +2995,7 @@
         <v>39</v>
       </c>
       <c r="AE16" t="s" s="2">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AF16" t="s" s="2">
         <v>40</v>
@@ -3033,10 +3004,10 @@
         <v>41</v>
       </c>
       <c r="AH16" t="s" s="2">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="AI16" t="s" s="2">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AJ16" t="s" s="2">
         <v>39</v>
@@ -3053,7 +3024,7 @@
         <v>91</v>
       </c>
       <c r="B17" t="s" s="2">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C17" t="s" s="2">
         <v>39</v>
@@ -3063,7 +3034,7 @@
         <v>40</v>
       </c>
       <c r="F17" t="s" s="2">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="G17" t="s" s="2">
         <v>48</v>
@@ -3075,13 +3046,13 @@
         <v>39</v>
       </c>
       <c r="J17" t="s" s="2">
+        <v>128</v>
+      </c>
+      <c r="K17" t="s" s="2">
         <v>129</v>
       </c>
-      <c r="K17" t="s" s="2">
+      <c r="L17" t="s" s="2">
         <v>130</v>
-      </c>
-      <c r="L17" t="s" s="2">
-        <v>131</v>
       </c>
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
@@ -3132,7 +3103,7 @@
         <v>39</v>
       </c>
       <c r="AE17" t="s" s="2">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AF17" t="s" s="2">
         <v>40</v>
@@ -3141,10 +3112,10 @@
         <v>41</v>
       </c>
       <c r="AH17" t="s" s="2">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="AI17" t="s" s="2">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AJ17" t="s" s="2">
         <v>39</v>
@@ -3156,15 +3127,13 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" hidden="true">
       <c r="A18" t="s" s="2">
-        <v>91</v>
-      </c>
-      <c r="B18" t="s" s="2">
+        <v>131</v>
+      </c>
+      <c r="B18" s="2"/>
+      <c r="C18" t="s" s="2">
         <v>132</v>
-      </c>
-      <c r="C18" t="s" s="2">
-        <v>39</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" t="s" s="2">
@@ -3174,25 +3143,29 @@
         <v>41</v>
       </c>
       <c r="G18" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="H18" t="s" s="2">
         <v>48</v>
       </c>
-      <c r="H18" t="s" s="2">
-        <v>39</v>
-      </c>
       <c r="I18" t="s" s="2">
         <v>39</v>
       </c>
       <c r="J18" t="s" s="2">
+        <v>92</v>
+      </c>
+      <c r="K18" t="s" s="2">
         <v>133</v>
       </c>
-      <c r="K18" t="s" s="2">
+      <c r="L18" t="s" s="2">
         <v>134</v>
       </c>
-      <c r="L18" t="s" s="2">
+      <c r="M18" t="s" s="2">
         <v>135</v>
       </c>
-      <c r="M18" s="2"/>
-      <c r="N18" s="2"/>
+      <c r="N18" t="s" s="2">
+        <v>136</v>
+      </c>
       <c r="O18" t="s" s="2">
         <v>39</v>
       </c>
@@ -3240,7 +3213,7 @@
         <v>39</v>
       </c>
       <c r="AE18" t="s" s="2">
-        <v>98</v>
+        <v>137</v>
       </c>
       <c r="AF18" t="s" s="2">
         <v>40</v>
@@ -3249,13 +3222,13 @@
         <v>41</v>
       </c>
       <c r="AH18" t="s" s="2">
-        <v>104</v>
+        <v>39</v>
       </c>
       <c r="AI18" t="s" s="2">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AJ18" t="s" s="2">
-        <v>39</v>
+        <v>90</v>
       </c>
       <c r="AK18" t="s" s="2">
         <v>39</v>
@@ -3266,17 +3239,15 @@
     </row>
     <row r="19">
       <c r="A19" t="s" s="2">
-        <v>91</v>
-      </c>
-      <c r="B19" t="s" s="2">
-        <v>136</v>
-      </c>
+        <v>138</v>
+      </c>
+      <c r="B19" s="2"/>
       <c r="C19" t="s" s="2">
         <v>39</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" t="s" s="2">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="F19" t="s" s="2">
         <v>47</v>
@@ -3288,16 +3259,16 @@
         <v>39</v>
       </c>
       <c r="I19" t="s" s="2">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="J19" t="s" s="2">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="K19" t="s" s="2">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="L19" t="s" s="2">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
@@ -3348,7 +3319,7 @@
         <v>39</v>
       </c>
       <c r="AE19" t="s" s="2">
-        <v>98</v>
+        <v>138</v>
       </c>
       <c r="AF19" t="s" s="2">
         <v>40</v>
@@ -3357,60 +3328,56 @@
         <v>41</v>
       </c>
       <c r="AH19" t="s" s="2">
-        <v>104</v>
+        <v>39</v>
       </c>
       <c r="AI19" t="s" s="2">
-        <v>99</v>
+        <v>59</v>
       </c>
       <c r="AJ19" t="s" s="2">
-        <v>39</v>
+        <v>142</v>
       </c>
       <c r="AK19" t="s" s="2">
-        <v>39</v>
+        <v>143</v>
       </c>
       <c r="AL19" t="s" s="2">
-        <v>39</v>
+        <v>144</v>
       </c>
     </row>
     <row r="20" hidden="true">
       <c r="A20" t="s" s="2">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" t="s" s="2">
-        <v>141</v>
+        <v>39</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" t="s" s="2">
         <v>40</v>
       </c>
       <c r="F20" t="s" s="2">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="G20" t="s" s="2">
         <v>39</v>
       </c>
       <c r="H20" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="I20" t="s" s="2">
         <v>48</v>
       </c>
-      <c r="I20" t="s" s="2">
-        <v>39</v>
-      </c>
       <c r="J20" t="s" s="2">
-        <v>93</v>
+        <v>139</v>
       </c>
       <c r="K20" t="s" s="2">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="L20" t="s" s="2">
-        <v>143</v>
-      </c>
-      <c r="M20" t="s" s="2">
-        <v>144</v>
-      </c>
-      <c r="N20" t="s" s="2">
-        <v>145</v>
-      </c>
+        <v>147</v>
+      </c>
+      <c r="M20" s="2"/>
+      <c r="N20" s="2"/>
       <c r="O20" t="s" s="2">
         <v>39</v>
       </c>
@@ -3458,33 +3425,33 @@
         <v>39</v>
       </c>
       <c r="AE20" t="s" s="2">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="AF20" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AG20" t="s" s="2">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="AH20" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AI20" t="s" s="2">
-        <v>99</v>
+        <v>59</v>
       </c>
       <c r="AJ20" t="s" s="2">
-        <v>90</v>
+        <v>148</v>
       </c>
       <c r="AK20" t="s" s="2">
-        <v>39</v>
+        <v>143</v>
       </c>
       <c r="AL20" t="s" s="2">
-        <v>39</v>
+        <v>149</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" hidden="true">
       <c r="A21" t="s" s="2">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" t="s" s="2">
@@ -3492,30 +3459,32 @@
       </c>
       <c r="D21" s="2"/>
       <c r="E21" t="s" s="2">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="F21" t="s" s="2">
         <v>47</v>
       </c>
       <c r="G21" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="H21" t="s" s="2">
         <v>48</v>
-      </c>
-      <c r="H21" t="s" s="2">
-        <v>39</v>
       </c>
       <c r="I21" t="s" s="2">
         <v>48</v>
       </c>
       <c r="J21" t="s" s="2">
-        <v>148</v>
+        <v>67</v>
       </c>
       <c r="K21" t="s" s="2">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="L21" t="s" s="2">
-        <v>150</v>
-      </c>
-      <c r="M21" s="2"/>
+        <v>152</v>
+      </c>
+      <c r="M21" t="s" s="2">
+        <v>153</v>
+      </c>
       <c r="N21" s="2"/>
       <c r="O21" t="s" s="2">
         <v>39</v>
@@ -3540,13 +3509,13 @@
         <v>39</v>
       </c>
       <c r="W21" t="s" s="2">
-        <v>39</v>
+        <v>154</v>
       </c>
       <c r="X21" t="s" s="2">
-        <v>39</v>
+        <v>155</v>
       </c>
       <c r="Y21" t="s" s="2">
-        <v>39</v>
+        <v>156</v>
       </c>
       <c r="Z21" t="s" s="2">
         <v>39</v>
@@ -3564,13 +3533,13 @@
         <v>39</v>
       </c>
       <c r="AE21" t="s" s="2">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="AF21" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AG21" t="s" s="2">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="AH21" t="s" s="2">
         <v>39</v>
@@ -3579,18 +3548,18 @@
         <v>59</v>
       </c>
       <c r="AJ21" t="s" s="2">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="AK21" t="s" s="2">
-        <v>152</v>
+        <v>158</v>
       </c>
       <c r="AL21" t="s" s="2">
-        <v>153</v>
+        <v>159</v>
       </c>
     </row>
-    <row r="22" hidden="true">
+    <row r="22">
       <c r="A22" t="s" s="2">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" t="s" s="2">
@@ -3604,7 +3573,7 @@
         <v>47</v>
       </c>
       <c r="G22" t="s" s="2">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="H22" t="s" s="2">
         <v>39</v>
@@ -3613,15 +3582,17 @@
         <v>48</v>
       </c>
       <c r="J22" t="s" s="2">
-        <v>148</v>
+        <v>161</v>
       </c>
       <c r="K22" t="s" s="2">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="L22" t="s" s="2">
-        <v>156</v>
-      </c>
-      <c r="M22" s="2"/>
+        <v>163</v>
+      </c>
+      <c r="M22" t="s" s="2">
+        <v>164</v>
+      </c>
       <c r="N22" s="2"/>
       <c r="O22" t="s" s="2">
         <v>39</v>
@@ -3646,13 +3617,13 @@
         <v>39</v>
       </c>
       <c r="W22" t="s" s="2">
-        <v>39</v>
+        <v>165</v>
       </c>
       <c r="X22" t="s" s="2">
-        <v>39</v>
+        <v>166</v>
       </c>
       <c r="Y22" t="s" s="2">
-        <v>39</v>
+        <v>167</v>
       </c>
       <c r="Z22" t="s" s="2">
         <v>39</v>
@@ -3670,7 +3641,7 @@
         <v>39</v>
       </c>
       <c r="AE22" t="s" s="2">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="AF22" t="s" s="2">
         <v>40</v>
@@ -3685,18 +3656,18 @@
         <v>59</v>
       </c>
       <c r="AJ22" t="s" s="2">
-        <v>157</v>
+        <v>168</v>
       </c>
       <c r="AK22" t="s" s="2">
-        <v>152</v>
+        <v>169</v>
       </c>
       <c r="AL22" t="s" s="2">
-        <v>158</v>
+        <v>170</v>
       </c>
     </row>
-    <row r="23" hidden="true">
+    <row r="23">
       <c r="A23" t="s" s="2">
-        <v>159</v>
+        <v>171</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" t="s" s="2">
@@ -3710,27 +3681,27 @@
         <v>47</v>
       </c>
       <c r="G23" t="s" s="2">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="H23" t="s" s="2">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="I23" t="s" s="2">
         <v>48</v>
       </c>
       <c r="J23" t="s" s="2">
-        <v>67</v>
+        <v>172</v>
       </c>
       <c r="K23" t="s" s="2">
-        <v>160</v>
+        <v>173</v>
       </c>
       <c r="L23" t="s" s="2">
-        <v>161</v>
-      </c>
-      <c r="M23" t="s" s="2">
-        <v>162</v>
-      </c>
-      <c r="N23" s="2"/>
+        <v>174</v>
+      </c>
+      <c r="M23" s="2"/>
+      <c r="N23" t="s" s="2">
+        <v>175</v>
+      </c>
       <c r="O23" t="s" s="2">
         <v>39</v>
       </c>
@@ -3754,13 +3725,13 @@
         <v>39</v>
       </c>
       <c r="W23" t="s" s="2">
-        <v>163</v>
+        <v>39</v>
       </c>
       <c r="X23" t="s" s="2">
-        <v>164</v>
+        <v>39</v>
       </c>
       <c r="Y23" t="s" s="2">
-        <v>165</v>
+        <v>39</v>
       </c>
       <c r="Z23" t="s" s="2">
         <v>39</v>
@@ -3778,7 +3749,7 @@
         <v>39</v>
       </c>
       <c r="AE23" t="s" s="2">
-        <v>159</v>
+        <v>171</v>
       </c>
       <c r="AF23" t="s" s="2">
         <v>40</v>
@@ -3793,18 +3764,18 @@
         <v>59</v>
       </c>
       <c r="AJ23" t="s" s="2">
-        <v>166</v>
+        <v>176</v>
       </c>
       <c r="AK23" t="s" s="2">
-        <v>167</v>
+        <v>177</v>
       </c>
       <c r="AL23" t="s" s="2">
-        <v>168</v>
+        <v>39</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
-        <v>169</v>
+        <v>178</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" t="s" s="2">
@@ -3818,7 +3789,7 @@
         <v>47</v>
       </c>
       <c r="G24" t="s" s="2">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="H24" t="s" s="2">
         <v>39</v>
@@ -3827,17 +3798,15 @@
         <v>48</v>
       </c>
       <c r="J24" t="s" s="2">
-        <v>170</v>
+        <v>179</v>
       </c>
       <c r="K24" t="s" s="2">
-        <v>171</v>
+        <v>180</v>
       </c>
       <c r="L24" t="s" s="2">
-        <v>172</v>
-      </c>
-      <c r="M24" t="s" s="2">
-        <v>173</v>
-      </c>
+        <v>181</v>
+      </c>
+      <c r="M24" s="2"/>
       <c r="N24" s="2"/>
       <c r="O24" t="s" s="2">
         <v>39</v>
@@ -3862,13 +3831,13 @@
         <v>39</v>
       </c>
       <c r="W24" t="s" s="2">
-        <v>174</v>
+        <v>39</v>
       </c>
       <c r="X24" t="s" s="2">
-        <v>175</v>
+        <v>39</v>
       </c>
       <c r="Y24" t="s" s="2">
-        <v>176</v>
+        <v>39</v>
       </c>
       <c r="Z24" t="s" s="2">
         <v>39</v>
@@ -3886,7 +3855,7 @@
         <v>39</v>
       </c>
       <c r="AE24" t="s" s="2">
-        <v>169</v>
+        <v>178</v>
       </c>
       <c r="AF24" t="s" s="2">
         <v>40</v>
@@ -3901,18 +3870,18 @@
         <v>59</v>
       </c>
       <c r="AJ24" t="s" s="2">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="AK24" t="s" s="2">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="AL24" t="s" s="2">
-        <v>179</v>
+        <v>184</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" hidden="true">
       <c r="A25" t="s" s="2">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" t="s" s="2">
@@ -3923,30 +3892,30 @@
         <v>40</v>
       </c>
       <c r="F25" t="s" s="2">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="G25" t="s" s="2">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="H25" t="s" s="2">
         <v>39</v>
       </c>
       <c r="I25" t="s" s="2">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="J25" t="s" s="2">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="K25" t="s" s="2">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="L25" t="s" s="2">
-        <v>183</v>
-      </c>
-      <c r="M25" s="2"/>
-      <c r="N25" t="s" s="2">
-        <v>184</v>
-      </c>
+        <v>188</v>
+      </c>
+      <c r="M25" t="s" s="2">
+        <v>189</v>
+      </c>
+      <c r="N25" s="2"/>
       <c r="O25" t="s" s="2">
         <v>39</v>
       </c>
@@ -3994,13 +3963,13 @@
         <v>39</v>
       </c>
       <c r="AE25" t="s" s="2">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="AF25" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AG25" t="s" s="2">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="AH25" t="s" s="2">
         <v>39</v>
@@ -4009,10 +3978,10 @@
         <v>59</v>
       </c>
       <c r="AJ25" t="s" s="2">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="AK25" t="s" s="2">
-        <v>186</v>
+        <v>39</v>
       </c>
       <c r="AL25" t="s" s="2">
         <v>39</v>
@@ -4020,7 +3989,7 @@
     </row>
     <row r="26" hidden="true">
       <c r="A26" t="s" s="2">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" t="s" s="2">
@@ -4031,7 +4000,7 @@
         <v>40</v>
       </c>
       <c r="F26" t="s" s="2">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="G26" t="s" s="2">
         <v>39</v>
@@ -4040,18 +4009,20 @@
         <v>39</v>
       </c>
       <c r="I26" t="s" s="2">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="J26" t="s" s="2">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="K26" t="s" s="2">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="L26" t="s" s="2">
-        <v>190</v>
-      </c>
-      <c r="M26" s="2"/>
+        <v>194</v>
+      </c>
+      <c r="M26" t="s" s="2">
+        <v>195</v>
+      </c>
       <c r="N26" s="2"/>
       <c r="O26" t="s" s="2">
         <v>39</v>
@@ -4100,13 +4071,13 @@
         <v>39</v>
       </c>
       <c r="AE26" t="s" s="2">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="AF26" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AG26" t="s" s="2">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="AH26" t="s" s="2">
         <v>39</v>
@@ -4115,18 +4086,18 @@
         <v>59</v>
       </c>
       <c r="AJ26" t="s" s="2">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="AK26" t="s" s="2">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="AL26" t="s" s="2">
-        <v>193</v>
+        <v>198</v>
       </c>
     </row>
     <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" t="s" s="2">
@@ -4137,7 +4108,7 @@
         <v>40</v>
       </c>
       <c r="F27" t="s" s="2">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="G27" t="s" s="2">
         <v>39</v>
@@ -4149,17 +4120,15 @@
         <v>39</v>
       </c>
       <c r="J27" t="s" s="2">
-        <v>195</v>
+        <v>200</v>
       </c>
       <c r="K27" t="s" s="2">
-        <v>196</v>
+        <v>201</v>
       </c>
       <c r="L27" t="s" s="2">
-        <v>197</v>
-      </c>
-      <c r="M27" t="s" s="2">
-        <v>198</v>
-      </c>
+        <v>202</v>
+      </c>
+      <c r="M27" s="2"/>
       <c r="N27" s="2"/>
       <c r="O27" t="s" s="2">
         <v>39</v>
@@ -4208,13 +4177,13 @@
         <v>39</v>
       </c>
       <c r="AE27" t="s" s="2">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="AF27" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AG27" t="s" s="2">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="AH27" t="s" s="2">
         <v>39</v>
@@ -4223,18 +4192,18 @@
         <v>59</v>
       </c>
       <c r="AJ27" t="s" s="2">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="AK27" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AL27" t="s" s="2">
-        <v>39</v>
+        <v>204</v>
       </c>
     </row>
     <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" t="s" s="2">
@@ -4245,7 +4214,7 @@
         <v>40</v>
       </c>
       <c r="F28" t="s" s="2">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="G28" t="s" s="2">
         <v>39</v>
@@ -4257,17 +4226,15 @@
         <v>39</v>
       </c>
       <c r="J28" t="s" s="2">
-        <v>201</v>
+        <v>49</v>
       </c>
       <c r="K28" t="s" s="2">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="L28" t="s" s="2">
-        <v>203</v>
-      </c>
-      <c r="M28" t="s" s="2">
-        <v>204</v>
-      </c>
+        <v>207</v>
+      </c>
+      <c r="M28" s="2"/>
       <c r="N28" s="2"/>
       <c r="O28" t="s" s="2">
         <v>39</v>
@@ -4316,44 +4283,44 @@
         <v>39</v>
       </c>
       <c r="AE28" t="s" s="2">
-        <v>200</v>
+        <v>208</v>
       </c>
       <c r="AF28" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AG28" t="s" s="2">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="AH28" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AI28" t="s" s="2">
-        <v>59</v>
+        <v>39</v>
       </c>
       <c r="AJ28" t="s" s="2">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="AK28" t="s" s="2">
-        <v>206</v>
+        <v>39</v>
       </c>
       <c r="AL28" t="s" s="2">
-        <v>207</v>
+        <v>39</v>
       </c>
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" t="s" s="2">
-        <v>39</v>
+        <v>132</v>
       </c>
       <c r="D29" s="2"/>
       <c r="E29" t="s" s="2">
         <v>40</v>
       </c>
       <c r="F29" t="s" s="2">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="G29" t="s" s="2">
         <v>39</v>
@@ -4365,15 +4332,17 @@
         <v>39</v>
       </c>
       <c r="J29" t="s" s="2">
-        <v>209</v>
+        <v>92</v>
       </c>
       <c r="K29" t="s" s="2">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="L29" t="s" s="2">
-        <v>211</v>
-      </c>
-      <c r="M29" s="2"/>
+        <v>212</v>
+      </c>
+      <c r="M29" t="s" s="2">
+        <v>135</v>
+      </c>
       <c r="N29" s="2"/>
       <c r="O29" t="s" s="2">
         <v>39</v>
@@ -4422,28 +4391,28 @@
         <v>39</v>
       </c>
       <c r="AE29" t="s" s="2">
-        <v>208</v>
+        <v>213</v>
       </c>
       <c r="AF29" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AG29" t="s" s="2">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="AH29" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AI29" t="s" s="2">
-        <v>59</v>
+        <v>98</v>
       </c>
       <c r="AJ29" t="s" s="2">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="AK29" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AL29" t="s" s="2">
-        <v>213</v>
+        <v>39</v>
       </c>
     </row>
     <row r="30" hidden="true">
@@ -4452,35 +4421,39 @@
       </c>
       <c r="B30" s="2"/>
       <c r="C30" t="s" s="2">
-        <v>39</v>
+        <v>215</v>
       </c>
       <c r="D30" s="2"/>
       <c r="E30" t="s" s="2">
         <v>40</v>
       </c>
       <c r="F30" t="s" s="2">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="G30" t="s" s="2">
         <v>39</v>
       </c>
       <c r="H30" t="s" s="2">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="I30" t="s" s="2">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="J30" t="s" s="2">
-        <v>49</v>
+        <v>92</v>
       </c>
       <c r="K30" t="s" s="2">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="L30" t="s" s="2">
-        <v>216</v>
-      </c>
-      <c r="M30" s="2"/>
-      <c r="N30" s="2"/>
+        <v>217</v>
+      </c>
+      <c r="M30" t="s" s="2">
+        <v>135</v>
+      </c>
+      <c r="N30" t="s" s="2">
+        <v>136</v>
+      </c>
       <c r="O30" t="s" s="2">
         <v>39</v>
       </c>
@@ -4528,22 +4501,22 @@
         <v>39</v>
       </c>
       <c r="AE30" t="s" s="2">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="AF30" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AG30" t="s" s="2">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="AH30" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AI30" t="s" s="2">
-        <v>39</v>
+        <v>98</v>
       </c>
       <c r="AJ30" t="s" s="2">
-        <v>218</v>
+        <v>90</v>
       </c>
       <c r="AK30" t="s" s="2">
         <v>39</v>
@@ -4558,14 +4531,14 @@
       </c>
       <c r="B31" s="2"/>
       <c r="C31" t="s" s="2">
-        <v>141</v>
+        <v>39</v>
       </c>
       <c r="D31" s="2"/>
       <c r="E31" t="s" s="2">
         <v>40</v>
       </c>
       <c r="F31" t="s" s="2">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="G31" t="s" s="2">
         <v>39</v>
@@ -4574,20 +4547,18 @@
         <v>39</v>
       </c>
       <c r="I31" t="s" s="2">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="J31" t="s" s="2">
-        <v>93</v>
+        <v>220</v>
       </c>
       <c r="K31" t="s" s="2">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>221</v>
-      </c>
-      <c r="M31" t="s" s="2">
-        <v>144</v>
-      </c>
+        <v>222</v>
+      </c>
+      <c r="M31" s="2"/>
       <c r="N31" s="2"/>
       <c r="O31" t="s" s="2">
         <v>39</v>
@@ -4636,69 +4607,65 @@
         <v>39</v>
       </c>
       <c r="AE31" t="s" s="2">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="AF31" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AG31" t="s" s="2">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="AH31" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AI31" t="s" s="2">
-        <v>99</v>
+        <v>59</v>
       </c>
       <c r="AJ31" t="s" s="2">
-        <v>218</v>
+        <v>223</v>
       </c>
       <c r="AK31" t="s" s="2">
-        <v>39</v>
+        <v>224</v>
       </c>
       <c r="AL31" t="s" s="2">
-        <v>39</v>
+        <v>225</v>
       </c>
     </row>
-    <row r="32" hidden="true">
+    <row r="32">
       <c r="A32" t="s" s="2">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" t="s" s="2">
-        <v>224</v>
+        <v>39</v>
       </c>
       <c r="D32" s="2"/>
       <c r="E32" t="s" s="2">
         <v>40</v>
       </c>
       <c r="F32" t="s" s="2">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="G32" t="s" s="2">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="H32" t="s" s="2">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="I32" t="s" s="2">
         <v>48</v>
       </c>
       <c r="J32" t="s" s="2">
-        <v>93</v>
+        <v>227</v>
       </c>
       <c r="K32" t="s" s="2">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>226</v>
-      </c>
-      <c r="M32" t="s" s="2">
-        <v>144</v>
-      </c>
-      <c r="N32" t="s" s="2">
-        <v>145</v>
-      </c>
+        <v>229</v>
+      </c>
+      <c r="M32" s="2"/>
+      <c r="N32" s="2"/>
       <c r="O32" t="s" s="2">
         <v>39</v>
       </c>
@@ -4746,33 +4713,33 @@
         <v>39</v>
       </c>
       <c r="AE32" t="s" s="2">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="AF32" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AG32" t="s" s="2">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="AH32" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AI32" t="s" s="2">
-        <v>99</v>
+        <v>59</v>
       </c>
       <c r="AJ32" t="s" s="2">
-        <v>90</v>
+        <v>230</v>
       </c>
       <c r="AK32" t="s" s="2">
-        <v>39</v>
+        <v>231</v>
       </c>
       <c r="AL32" t="s" s="2">
-        <v>39</v>
+        <v>232</v>
       </c>
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>228</v>
+        <v>233</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" t="s" s="2">
@@ -4795,13 +4762,13 @@
         <v>48</v>
       </c>
       <c r="J33" t="s" s="2">
-        <v>229</v>
+        <v>234</v>
       </c>
       <c r="K33" t="s" s="2">
-        <v>230</v>
+        <v>235</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>231</v>
+        <v>236</v>
       </c>
       <c r="M33" s="2"/>
       <c r="N33" s="2"/>
@@ -4852,7 +4819,7 @@
         <v>39</v>
       </c>
       <c r="AE33" t="s" s="2">
-        <v>228</v>
+        <v>233</v>
       </c>
       <c r="AF33" t="s" s="2">
         <v>40</v>
@@ -4867,18 +4834,18 @@
         <v>59</v>
       </c>
       <c r="AJ33" t="s" s="2">
-        <v>232</v>
+        <v>39</v>
       </c>
       <c r="AK33" t="s" s="2">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="AL33" t="s" s="2">
-        <v>234</v>
+        <v>39</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" t="s" s="2">
@@ -4892,22 +4859,22 @@
         <v>47</v>
       </c>
       <c r="G34" t="s" s="2">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="H34" t="s" s="2">
         <v>39</v>
       </c>
       <c r="I34" t="s" s="2">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="J34" t="s" s="2">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="K34" t="s" s="2">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
@@ -4958,7 +4925,7 @@
         <v>39</v>
       </c>
       <c r="AE34" t="s" s="2">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="AF34" t="s" s="2">
         <v>40</v>
@@ -4973,18 +4940,18 @@
         <v>59</v>
       </c>
       <c r="AJ34" t="s" s="2">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="AK34" t="s" s="2">
-        <v>240</v>
+        <v>39</v>
       </c>
       <c r="AL34" t="s" s="2">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" t="s" s="2">
@@ -5004,10 +4971,10 @@
         <v>39</v>
       </c>
       <c r="I35" t="s" s="2">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="J35" t="s" s="2">
-        <v>243</v>
+        <v>161</v>
       </c>
       <c r="K35" t="s" s="2">
         <v>244</v>
@@ -5040,13 +5007,13 @@
         <v>39</v>
       </c>
       <c r="W35" t="s" s="2">
-        <v>39</v>
+        <v>165</v>
       </c>
       <c r="X35" t="s" s="2">
-        <v>39</v>
+        <v>246</v>
       </c>
       <c r="Y35" t="s" s="2">
-        <v>39</v>
+        <v>247</v>
       </c>
       <c r="Z35" t="s" s="2">
         <v>39</v>
@@ -5064,7 +5031,7 @@
         <v>39</v>
       </c>
       <c r="AE35" t="s" s="2">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="AF35" t="s" s="2">
         <v>40</v>
@@ -5079,18 +5046,18 @@
         <v>59</v>
       </c>
       <c r="AJ35" t="s" s="2">
-        <v>39</v>
+        <v>248</v>
       </c>
       <c r="AK35" t="s" s="2">
-        <v>240</v>
+        <v>39</v>
       </c>
       <c r="AL35" t="s" s="2">
-        <v>39</v>
+        <v>249</v>
       </c>
     </row>
-    <row r="36" hidden="true">
+    <row r="36">
       <c r="A36" t="s" s="2">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" t="s" s="2">
@@ -5104,7 +5071,7 @@
         <v>47</v>
       </c>
       <c r="G36" t="s" s="2">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="H36" t="s" s="2">
         <v>39</v>
@@ -5113,15 +5080,17 @@
         <v>39</v>
       </c>
       <c r="J36" t="s" s="2">
-        <v>247</v>
+        <v>161</v>
       </c>
       <c r="K36" t="s" s="2">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>249</v>
-      </c>
-      <c r="M36" s="2"/>
+        <v>252</v>
+      </c>
+      <c r="M36" t="s" s="2">
+        <v>253</v>
+      </c>
       <c r="N36" s="2"/>
       <c r="O36" t="s" s="2">
         <v>39</v>
@@ -5146,13 +5115,13 @@
         <v>39</v>
       </c>
       <c r="W36" t="s" s="2">
-        <v>39</v>
+        <v>165</v>
       </c>
       <c r="X36" t="s" s="2">
-        <v>39</v>
+        <v>254</v>
       </c>
       <c r="Y36" t="s" s="2">
-        <v>39</v>
+        <v>255</v>
       </c>
       <c r="Z36" t="s" s="2">
         <v>39</v>
@@ -5170,7 +5139,7 @@
         <v>39</v>
       </c>
       <c r="AE36" t="s" s="2">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="AF36" t="s" s="2">
         <v>40</v>
@@ -5185,18 +5154,18 @@
         <v>59</v>
       </c>
       <c r="AJ36" t="s" s="2">
-        <v>250</v>
+        <v>256</v>
       </c>
       <c r="AK36" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AL36" t="s" s="2">
-        <v>251</v>
+        <v>257</v>
       </c>
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" t="s" s="2">
@@ -5216,19 +5185,23 @@
         <v>39</v>
       </c>
       <c r="I37" t="s" s="2">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="J37" t="s" s="2">
-        <v>170</v>
+        <v>259</v>
       </c>
       <c r="K37" t="s" s="2">
-        <v>253</v>
+        <v>260</v>
       </c>
       <c r="L37" t="s" s="2">
-        <v>254</v>
-      </c>
-      <c r="M37" s="2"/>
-      <c r="N37" s="2"/>
+        <v>261</v>
+      </c>
+      <c r="M37" t="s" s="2">
+        <v>262</v>
+      </c>
+      <c r="N37" t="s" s="2">
+        <v>263</v>
+      </c>
       <c r="O37" t="s" s="2">
         <v>39</v>
       </c>
@@ -5252,13 +5225,13 @@
         <v>39</v>
       </c>
       <c r="W37" t="s" s="2">
-        <v>174</v>
+        <v>264</v>
       </c>
       <c r="X37" t="s" s="2">
-        <v>255</v>
+        <v>265</v>
       </c>
       <c r="Y37" t="s" s="2">
-        <v>256</v>
+        <v>266</v>
       </c>
       <c r="Z37" t="s" s="2">
         <v>39</v>
@@ -5276,7 +5249,7 @@
         <v>39</v>
       </c>
       <c r="AE37" t="s" s="2">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="AF37" t="s" s="2">
         <v>40</v>
@@ -5291,18 +5264,18 @@
         <v>59</v>
       </c>
       <c r="AJ37" t="s" s="2">
-        <v>257</v>
+        <v>39</v>
       </c>
       <c r="AK37" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AL37" t="s" s="2">
-        <v>258</v>
+        <v>267</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>259</v>
+        <v>268</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" t="s" s="2">
@@ -5313,10 +5286,10 @@
         <v>40</v>
       </c>
       <c r="F38" t="s" s="2">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="G38" t="s" s="2">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="H38" t="s" s="2">
         <v>39</v>
@@ -5325,17 +5298,15 @@
         <v>39</v>
       </c>
       <c r="J38" t="s" s="2">
-        <v>170</v>
+        <v>200</v>
       </c>
       <c r="K38" t="s" s="2">
-        <v>260</v>
+        <v>269</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>261</v>
-      </c>
-      <c r="M38" t="s" s="2">
-        <v>262</v>
-      </c>
+        <v>270</v>
+      </c>
+      <c r="M38" s="2"/>
       <c r="N38" s="2"/>
       <c r="O38" t="s" s="2">
         <v>39</v>
@@ -5360,13 +5331,13 @@
         <v>39</v>
       </c>
       <c r="W38" t="s" s="2">
-        <v>174</v>
+        <v>39</v>
       </c>
       <c r="X38" t="s" s="2">
-        <v>263</v>
+        <v>39</v>
       </c>
       <c r="Y38" t="s" s="2">
-        <v>264</v>
+        <v>39</v>
       </c>
       <c r="Z38" t="s" s="2">
         <v>39</v>
@@ -5384,13 +5355,13 @@
         <v>39</v>
       </c>
       <c r="AE38" t="s" s="2">
-        <v>259</v>
+        <v>268</v>
       </c>
       <c r="AF38" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AG38" t="s" s="2">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="AH38" t="s" s="2">
         <v>39</v>
@@ -5399,18 +5370,18 @@
         <v>59</v>
       </c>
       <c r="AJ38" t="s" s="2">
-        <v>265</v>
+        <v>271</v>
       </c>
       <c r="AK38" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AL38" t="s" s="2">
-        <v>266</v>
+        <v>39</v>
       </c>
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>267</v>
+        <v>272</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" t="s" s="2">
@@ -5430,23 +5401,19 @@
         <v>39</v>
       </c>
       <c r="I39" t="s" s="2">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="J39" t="s" s="2">
-        <v>268</v>
+        <v>49</v>
       </c>
       <c r="K39" t="s" s="2">
-        <v>269</v>
+        <v>206</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>270</v>
-      </c>
-      <c r="M39" t="s" s="2">
-        <v>271</v>
-      </c>
-      <c r="N39" t="s" s="2">
-        <v>272</v>
-      </c>
+        <v>207</v>
+      </c>
+      <c r="M39" s="2"/>
+      <c r="N39" s="2"/>
       <c r="O39" t="s" s="2">
         <v>39</v>
       </c>
@@ -5470,13 +5437,13 @@
         <v>39</v>
       </c>
       <c r="W39" t="s" s="2">
-        <v>273</v>
+        <v>39</v>
       </c>
       <c r="X39" t="s" s="2">
-        <v>274</v>
+        <v>39</v>
       </c>
       <c r="Y39" t="s" s="2">
-        <v>275</v>
+        <v>39</v>
       </c>
       <c r="Z39" t="s" s="2">
         <v>39</v>
@@ -5494,7 +5461,7 @@
         <v>39</v>
       </c>
       <c r="AE39" t="s" s="2">
-        <v>267</v>
+        <v>208</v>
       </c>
       <c r="AF39" t="s" s="2">
         <v>40</v>
@@ -5506,25 +5473,25 @@
         <v>39</v>
       </c>
       <c r="AI39" t="s" s="2">
-        <v>59</v>
+        <v>39</v>
       </c>
       <c r="AJ39" t="s" s="2">
-        <v>39</v>
+        <v>209</v>
       </c>
       <c r="AK39" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AL39" t="s" s="2">
-        <v>276</v>
+        <v>39</v>
       </c>
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" t="s" s="2">
-        <v>39</v>
+        <v>132</v>
       </c>
       <c r="D40" s="2"/>
       <c r="E40" t="s" s="2">
@@ -5543,15 +5510,17 @@
         <v>39</v>
       </c>
       <c r="J40" t="s" s="2">
-        <v>209</v>
+        <v>92</v>
       </c>
       <c r="K40" t="s" s="2">
-        <v>278</v>
+        <v>211</v>
       </c>
       <c r="L40" t="s" s="2">
-        <v>279</v>
-      </c>
-      <c r="M40" s="2"/>
+        <v>212</v>
+      </c>
+      <c r="M40" t="s" s="2">
+        <v>135</v>
+      </c>
       <c r="N40" s="2"/>
       <c r="O40" t="s" s="2">
         <v>39</v>
@@ -5600,7 +5569,7 @@
         <v>39</v>
       </c>
       <c r="AE40" t="s" s="2">
-        <v>277</v>
+        <v>213</v>
       </c>
       <c r="AF40" t="s" s="2">
         <v>40</v>
@@ -5612,10 +5581,10 @@
         <v>39</v>
       </c>
       <c r="AI40" t="s" s="2">
-        <v>59</v>
+        <v>98</v>
       </c>
       <c r="AJ40" t="s" s="2">
-        <v>280</v>
+        <v>209</v>
       </c>
       <c r="AK40" t="s" s="2">
         <v>39</v>
@@ -5626,39 +5595,43 @@
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" t="s" s="2">
-        <v>39</v>
+        <v>215</v>
       </c>
       <c r="D41" s="2"/>
       <c r="E41" t="s" s="2">
         <v>40</v>
       </c>
       <c r="F41" t="s" s="2">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="G41" t="s" s="2">
         <v>39</v>
       </c>
       <c r="H41" t="s" s="2">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="I41" t="s" s="2">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="J41" t="s" s="2">
-        <v>49</v>
+        <v>92</v>
       </c>
       <c r="K41" t="s" s="2">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="L41" t="s" s="2">
-        <v>216</v>
-      </c>
-      <c r="M41" s="2"/>
-      <c r="N41" s="2"/>
+        <v>217</v>
+      </c>
+      <c r="M41" t="s" s="2">
+        <v>135</v>
+      </c>
+      <c r="N41" t="s" s="2">
+        <v>136</v>
+      </c>
       <c r="O41" t="s" s="2">
         <v>39</v>
       </c>
@@ -5706,22 +5679,22 @@
         <v>39</v>
       </c>
       <c r="AE41" t="s" s="2">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="AF41" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AG41" t="s" s="2">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="AH41" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AI41" t="s" s="2">
-        <v>39</v>
+        <v>98</v>
       </c>
       <c r="AJ41" t="s" s="2">
-        <v>218</v>
+        <v>90</v>
       </c>
       <c r="AK41" t="s" s="2">
         <v>39</v>
@@ -5732,18 +5705,18 @@
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" t="s" s="2">
-        <v>141</v>
+        <v>39</v>
       </c>
       <c r="D42" s="2"/>
       <c r="E42" t="s" s="2">
         <v>40</v>
       </c>
       <c r="F42" t="s" s="2">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="G42" t="s" s="2">
         <v>39</v>
@@ -5755,17 +5728,15 @@
         <v>39</v>
       </c>
       <c r="J42" t="s" s="2">
-        <v>93</v>
+        <v>49</v>
       </c>
       <c r="K42" t="s" s="2">
-        <v>220</v>
+        <v>276</v>
       </c>
       <c r="L42" t="s" s="2">
-        <v>221</v>
-      </c>
-      <c r="M42" t="s" s="2">
-        <v>144</v>
-      </c>
+        <v>277</v>
+      </c>
+      <c r="M42" s="2"/>
       <c r="N42" s="2"/>
       <c r="O42" t="s" s="2">
         <v>39</v>
@@ -5814,22 +5785,22 @@
         <v>39</v>
       </c>
       <c r="AE42" t="s" s="2">
-        <v>222</v>
+        <v>275</v>
       </c>
       <c r="AF42" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AG42" t="s" s="2">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="AH42" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AI42" t="s" s="2">
-        <v>99</v>
+        <v>59</v>
       </c>
       <c r="AJ42" t="s" s="2">
-        <v>218</v>
+        <v>278</v>
       </c>
       <c r="AK42" t="s" s="2">
         <v>39</v>
@@ -5838,45 +5809,41 @@
         <v>39</v>
       </c>
     </row>
-    <row r="43" hidden="true">
+    <row r="43">
       <c r="A43" t="s" s="2">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" t="s" s="2">
-        <v>224</v>
+        <v>39</v>
       </c>
       <c r="D43" s="2"/>
       <c r="E43" t="s" s="2">
         <v>40</v>
       </c>
       <c r="F43" t="s" s="2">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="G43" t="s" s="2">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="H43" t="s" s="2">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="I43" t="s" s="2">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="J43" t="s" s="2">
-        <v>93</v>
+        <v>161</v>
       </c>
       <c r="K43" t="s" s="2">
-        <v>225</v>
+        <v>280</v>
       </c>
       <c r="L43" t="s" s="2">
-        <v>226</v>
-      </c>
-      <c r="M43" t="s" s="2">
-        <v>144</v>
-      </c>
-      <c r="N43" t="s" s="2">
-        <v>145</v>
-      </c>
+        <v>281</v>
+      </c>
+      <c r="M43" s="2"/>
+      <c r="N43" s="2"/>
       <c r="O43" t="s" s="2">
         <v>39</v>
       </c>
@@ -5900,13 +5867,13 @@
         <v>39</v>
       </c>
       <c r="W43" t="s" s="2">
-        <v>39</v>
+        <v>165</v>
       </c>
       <c r="X43" t="s" s="2">
-        <v>39</v>
+        <v>282</v>
       </c>
       <c r="Y43" t="s" s="2">
-        <v>39</v>
+        <v>283</v>
       </c>
       <c r="Z43" t="s" s="2">
         <v>39</v>
@@ -5924,22 +5891,22 @@
         <v>39</v>
       </c>
       <c r="AE43" t="s" s="2">
-        <v>227</v>
+        <v>279</v>
       </c>
       <c r="AF43" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AG43" t="s" s="2">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="AH43" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AI43" t="s" s="2">
-        <v>99</v>
+        <v>59</v>
       </c>
       <c r="AJ43" t="s" s="2">
-        <v>90</v>
+        <v>168</v>
       </c>
       <c r="AK43" t="s" s="2">
         <v>39</v>
@@ -5961,7 +5928,7 @@
         <v>40</v>
       </c>
       <c r="F44" t="s" s="2">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="G44" t="s" s="2">
         <v>39</v>
@@ -5973,13 +5940,13 @@
         <v>39</v>
       </c>
       <c r="J44" t="s" s="2">
-        <v>49</v>
+        <v>285</v>
       </c>
       <c r="K44" t="s" s="2">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="L44" t="s" s="2">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="M44" s="2"/>
       <c r="N44" s="2"/>
@@ -6036,7 +6003,7 @@
         <v>40</v>
       </c>
       <c r="AG44" t="s" s="2">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="AH44" t="s" s="2">
         <v>39</v>
@@ -6045,18 +6012,18 @@
         <v>59</v>
       </c>
       <c r="AJ44" t="s" s="2">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="AK44" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AL44" t="s" s="2">
-        <v>39</v>
+        <v>289</v>
       </c>
     </row>
-    <row r="45">
+    <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" t="s" s="2">
@@ -6070,7 +6037,7 @@
         <v>47</v>
       </c>
       <c r="G45" t="s" s="2">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="H45" t="s" s="2">
         <v>39</v>
@@ -6079,13 +6046,13 @@
         <v>39</v>
       </c>
       <c r="J45" t="s" s="2">
-        <v>170</v>
+        <v>227</v>
       </c>
       <c r="K45" t="s" s="2">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="L45" t="s" s="2">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="M45" s="2"/>
       <c r="N45" s="2"/>
@@ -6112,13 +6079,13 @@
         <v>39</v>
       </c>
       <c r="W45" t="s" s="2">
-        <v>174</v>
+        <v>39</v>
       </c>
       <c r="X45" t="s" s="2">
-        <v>291</v>
+        <v>39</v>
       </c>
       <c r="Y45" t="s" s="2">
-        <v>292</v>
+        <v>39</v>
       </c>
       <c r="Z45" t="s" s="2">
         <v>39</v>
@@ -6136,7 +6103,7 @@
         <v>39</v>
       </c>
       <c r="AE45" t="s" s="2">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="AF45" t="s" s="2">
         <v>40</v>
@@ -6151,7 +6118,7 @@
         <v>59</v>
       </c>
       <c r="AJ45" t="s" s="2">
-        <v>177</v>
+        <v>230</v>
       </c>
       <c r="AK45" t="s" s="2">
         <v>39</v>
@@ -6185,13 +6152,13 @@
         <v>39</v>
       </c>
       <c r="J46" t="s" s="2">
+        <v>200</v>
+      </c>
+      <c r="K46" t="s" s="2">
         <v>294</v>
       </c>
-      <c r="K46" t="s" s="2">
+      <c r="L46" t="s" s="2">
         <v>295</v>
-      </c>
-      <c r="L46" t="s" s="2">
-        <v>296</v>
       </c>
       <c r="M46" s="2"/>
       <c r="N46" s="2"/>
@@ -6257,18 +6224,18 @@
         <v>59</v>
       </c>
       <c r="AJ46" t="s" s="2">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="AK46" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AL46" t="s" s="2">
-        <v>298</v>
+        <v>39</v>
       </c>
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" t="s" s="2">
@@ -6291,13 +6258,13 @@
         <v>39</v>
       </c>
       <c r="J47" t="s" s="2">
-        <v>236</v>
+        <v>49</v>
       </c>
       <c r="K47" t="s" s="2">
-        <v>300</v>
+        <v>206</v>
       </c>
       <c r="L47" t="s" s="2">
-        <v>301</v>
+        <v>207</v>
       </c>
       <c r="M47" s="2"/>
       <c r="N47" s="2"/>
@@ -6348,7 +6315,7 @@
         <v>39</v>
       </c>
       <c r="AE47" t="s" s="2">
-        <v>299</v>
+        <v>208</v>
       </c>
       <c r="AF47" t="s" s="2">
         <v>40</v>
@@ -6360,10 +6327,10 @@
         <v>39</v>
       </c>
       <c r="AI47" t="s" s="2">
-        <v>59</v>
+        <v>39</v>
       </c>
       <c r="AJ47" t="s" s="2">
-        <v>239</v>
+        <v>209</v>
       </c>
       <c r="AK47" t="s" s="2">
         <v>39</v>
@@ -6374,11 +6341,11 @@
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" t="s" s="2">
-        <v>39</v>
+        <v>132</v>
       </c>
       <c r="D48" s="2"/>
       <c r="E48" t="s" s="2">
@@ -6397,15 +6364,17 @@
         <v>39</v>
       </c>
       <c r="J48" t="s" s="2">
-        <v>209</v>
+        <v>92</v>
       </c>
       <c r="K48" t="s" s="2">
-        <v>303</v>
+        <v>211</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>304</v>
-      </c>
-      <c r="M48" s="2"/>
+        <v>212</v>
+      </c>
+      <c r="M48" t="s" s="2">
+        <v>135</v>
+      </c>
       <c r="N48" s="2"/>
       <c r="O48" t="s" s="2">
         <v>39</v>
@@ -6454,7 +6423,7 @@
         <v>39</v>
       </c>
       <c r="AE48" t="s" s="2">
-        <v>302</v>
+        <v>213</v>
       </c>
       <c r="AF48" t="s" s="2">
         <v>40</v>
@@ -6466,10 +6435,10 @@
         <v>39</v>
       </c>
       <c r="AI48" t="s" s="2">
-        <v>59</v>
+        <v>98</v>
       </c>
       <c r="AJ48" t="s" s="2">
-        <v>305</v>
+        <v>209</v>
       </c>
       <c r="AK48" t="s" s="2">
         <v>39</v>
@@ -6480,39 +6449,43 @@
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>306</v>
+        <v>299</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" t="s" s="2">
-        <v>39</v>
+        <v>215</v>
       </c>
       <c r="D49" s="2"/>
       <c r="E49" t="s" s="2">
         <v>40</v>
       </c>
       <c r="F49" t="s" s="2">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="G49" t="s" s="2">
         <v>39</v>
       </c>
       <c r="H49" t="s" s="2">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="I49" t="s" s="2">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="J49" t="s" s="2">
-        <v>49</v>
+        <v>92</v>
       </c>
       <c r="K49" t="s" s="2">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="L49" t="s" s="2">
-        <v>216</v>
-      </c>
-      <c r="M49" s="2"/>
-      <c r="N49" s="2"/>
+        <v>217</v>
+      </c>
+      <c r="M49" t="s" s="2">
+        <v>135</v>
+      </c>
+      <c r="N49" t="s" s="2">
+        <v>136</v>
+      </c>
       <c r="O49" t="s" s="2">
         <v>39</v>
       </c>
@@ -6560,22 +6533,22 @@
         <v>39</v>
       </c>
       <c r="AE49" t="s" s="2">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="AF49" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AG49" t="s" s="2">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="AH49" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AI49" t="s" s="2">
-        <v>39</v>
+        <v>98</v>
       </c>
       <c r="AJ49" t="s" s="2">
-        <v>218</v>
+        <v>90</v>
       </c>
       <c r="AK49" t="s" s="2">
         <v>39</v>
@@ -6586,11 +6559,11 @@
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>307</v>
+        <v>300</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" t="s" s="2">
-        <v>141</v>
+        <v>39</v>
       </c>
       <c r="D50" s="2"/>
       <c r="E50" t="s" s="2">
@@ -6606,20 +6579,18 @@
         <v>39</v>
       </c>
       <c r="I50" t="s" s="2">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="J50" t="s" s="2">
-        <v>93</v>
+        <v>139</v>
       </c>
       <c r="K50" t="s" s="2">
-        <v>220</v>
+        <v>301</v>
       </c>
       <c r="L50" t="s" s="2">
-        <v>221</v>
-      </c>
-      <c r="M50" t="s" s="2">
-        <v>144</v>
-      </c>
+        <v>302</v>
+      </c>
+      <c r="M50" s="2"/>
       <c r="N50" s="2"/>
       <c r="O50" t="s" s="2">
         <v>39</v>
@@ -6668,7 +6639,7 @@
         <v>39</v>
       </c>
       <c r="AE50" t="s" s="2">
-        <v>222</v>
+        <v>300</v>
       </c>
       <c r="AF50" t="s" s="2">
         <v>40</v>
@@ -6680,57 +6651,53 @@
         <v>39</v>
       </c>
       <c r="AI50" t="s" s="2">
-        <v>99</v>
+        <v>59</v>
       </c>
       <c r="AJ50" t="s" s="2">
-        <v>218</v>
+        <v>142</v>
       </c>
       <c r="AK50" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AL50" t="s" s="2">
-        <v>39</v>
+        <v>303</v>
       </c>
     </row>
     <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" t="s" s="2">
-        <v>224</v>
+        <v>39</v>
       </c>
       <c r="D51" s="2"/>
       <c r="E51" t="s" s="2">
         <v>40</v>
       </c>
       <c r="F51" t="s" s="2">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="G51" t="s" s="2">
         <v>39</v>
       </c>
       <c r="H51" t="s" s="2">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="I51" t="s" s="2">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="J51" t="s" s="2">
-        <v>93</v>
+        <v>49</v>
       </c>
       <c r="K51" t="s" s="2">
-        <v>225</v>
+        <v>305</v>
       </c>
       <c r="L51" t="s" s="2">
-        <v>226</v>
-      </c>
-      <c r="M51" t="s" s="2">
-        <v>144</v>
-      </c>
-      <c r="N51" t="s" s="2">
-        <v>145</v>
-      </c>
+        <v>306</v>
+      </c>
+      <c r="M51" s="2"/>
+      <c r="N51" s="2"/>
       <c r="O51" t="s" s="2">
         <v>39</v>
       </c>
@@ -6778,22 +6745,22 @@
         <v>39</v>
       </c>
       <c r="AE51" t="s" s="2">
-        <v>227</v>
+        <v>304</v>
       </c>
       <c r="AF51" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AG51" t="s" s="2">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="AH51" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AI51" t="s" s="2">
-        <v>99</v>
+        <v>59</v>
       </c>
       <c r="AJ51" t="s" s="2">
-        <v>90</v>
+        <v>307</v>
       </c>
       <c r="AK51" t="s" s="2">
         <v>39</v>
@@ -6804,7 +6771,7 @@
     </row>
     <row r="52" hidden="true">
       <c r="A52" t="s" s="2">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" t="s" s="2">
@@ -6815,7 +6782,7 @@
         <v>40</v>
       </c>
       <c r="F52" t="s" s="2">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="G52" t="s" s="2">
         <v>39</v>
@@ -6824,16 +6791,16 @@
         <v>39</v>
       </c>
       <c r="I52" t="s" s="2">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="J52" t="s" s="2">
-        <v>148</v>
+        <v>161</v>
       </c>
       <c r="K52" t="s" s="2">
+        <v>309</v>
+      </c>
+      <c r="L52" t="s" s="2">
         <v>310</v>
-      </c>
-      <c r="L52" t="s" s="2">
-        <v>311</v>
       </c>
       <c r="M52" s="2"/>
       <c r="N52" s="2"/>
@@ -6860,13 +6827,13 @@
         <v>39</v>
       </c>
       <c r="W52" t="s" s="2">
-        <v>39</v>
+        <v>165</v>
       </c>
       <c r="X52" t="s" s="2">
-        <v>39</v>
+        <v>311</v>
       </c>
       <c r="Y52" t="s" s="2">
-        <v>39</v>
+        <v>312</v>
       </c>
       <c r="Z52" t="s" s="2">
         <v>39</v>
@@ -6884,13 +6851,13 @@
         <v>39</v>
       </c>
       <c r="AE52" t="s" s="2">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="AF52" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AG52" t="s" s="2">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="AH52" t="s" s="2">
         <v>39</v>
@@ -6899,18 +6866,18 @@
         <v>59</v>
       </c>
       <c r="AJ52" t="s" s="2">
-        <v>151</v>
+        <v>168</v>
       </c>
       <c r="AK52" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AL52" t="s" s="2">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row r="53" hidden="true">
       <c r="A53" t="s" s="2">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="B53" s="2"/>
       <c r="C53" t="s" s="2">
@@ -6933,13 +6900,13 @@
         <v>39</v>
       </c>
       <c r="J53" t="s" s="2">
-        <v>49</v>
+        <v>238</v>
       </c>
       <c r="K53" t="s" s="2">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="L53" t="s" s="2">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="M53" s="2"/>
       <c r="N53" s="2"/>
@@ -6990,7 +6957,7 @@
         <v>39</v>
       </c>
       <c r="AE53" t="s" s="2">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="AF53" t="s" s="2">
         <v>40</v>
@@ -7005,18 +6972,18 @@
         <v>59</v>
       </c>
       <c r="AJ53" t="s" s="2">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="AK53" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AL53" t="s" s="2">
-        <v>39</v>
+        <v>318</v>
       </c>
     </row>
     <row r="54" hidden="true">
       <c r="A54" t="s" s="2">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="B54" s="2"/>
       <c r="C54" t="s" s="2">
@@ -7039,13 +7006,13 @@
         <v>39</v>
       </c>
       <c r="J54" t="s" s="2">
-        <v>170</v>
+        <v>238</v>
       </c>
       <c r="K54" t="s" s="2">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="L54" t="s" s="2">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="M54" s="2"/>
       <c r="N54" s="2"/>
@@ -7072,13 +7039,13 @@
         <v>39</v>
       </c>
       <c r="W54" t="s" s="2">
-        <v>174</v>
+        <v>39</v>
       </c>
       <c r="X54" t="s" s="2">
-        <v>320</v>
+        <v>39</v>
       </c>
       <c r="Y54" t="s" s="2">
-        <v>321</v>
+        <v>39</v>
       </c>
       <c r="Z54" t="s" s="2">
         <v>39</v>
@@ -7096,7 +7063,7 @@
         <v>39</v>
       </c>
       <c r="AE54" t="s" s="2">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="AF54" t="s" s="2">
         <v>40</v>
@@ -7111,18 +7078,18 @@
         <v>59</v>
       </c>
       <c r="AJ54" t="s" s="2">
-        <v>177</v>
+        <v>322</v>
       </c>
       <c r="AK54" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AL54" t="s" s="2">
-        <v>322</v>
+        <v>323</v>
       </c>
     </row>
     <row r="55" hidden="true">
       <c r="A55" t="s" s="2">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="B55" s="2"/>
       <c r="C55" t="s" s="2">
@@ -7145,13 +7112,13 @@
         <v>39</v>
       </c>
       <c r="J55" t="s" s="2">
-        <v>247</v>
+        <v>325</v>
       </c>
       <c r="K55" t="s" s="2">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="L55" t="s" s="2">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="M55" s="2"/>
       <c r="N55" s="2"/>
@@ -7178,13 +7145,13 @@
         <v>39</v>
       </c>
       <c r="W55" t="s" s="2">
-        <v>39</v>
+        <v>165</v>
       </c>
       <c r="X55" t="s" s="2">
-        <v>39</v>
+        <v>328</v>
       </c>
       <c r="Y55" t="s" s="2">
-        <v>39</v>
+        <v>329</v>
       </c>
       <c r="Z55" t="s" s="2">
         <v>39</v>
@@ -7202,7 +7169,7 @@
         <v>39</v>
       </c>
       <c r="AE55" t="s" s="2">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="AF55" t="s" s="2">
         <v>40</v>
@@ -7217,18 +7184,18 @@
         <v>59</v>
       </c>
       <c r="AJ55" t="s" s="2">
-        <v>326</v>
+        <v>330</v>
       </c>
       <c r="AK55" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AL55" t="s" s="2">
-        <v>327</v>
+        <v>331</v>
       </c>
     </row>
     <row r="56" hidden="true">
       <c r="A56" t="s" s="2">
-        <v>328</v>
+        <v>332</v>
       </c>
       <c r="B56" s="2"/>
       <c r="C56" t="s" s="2">
@@ -7239,7 +7206,7 @@
         <v>40</v>
       </c>
       <c r="F56" t="s" s="2">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="G56" t="s" s="2">
         <v>39</v>
@@ -7248,19 +7215,23 @@
         <v>39</v>
       </c>
       <c r="I56" t="s" s="2">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="J56" t="s" s="2">
-        <v>247</v>
+        <v>161</v>
       </c>
       <c r="K56" t="s" s="2">
-        <v>329</v>
+        <v>333</v>
       </c>
       <c r="L56" t="s" s="2">
-        <v>330</v>
-      </c>
-      <c r="M56" s="2"/>
-      <c r="N56" s="2"/>
+        <v>334</v>
+      </c>
+      <c r="M56" t="s" s="2">
+        <v>335</v>
+      </c>
+      <c r="N56" t="s" s="2">
+        <v>336</v>
+      </c>
       <c r="O56" t="s" s="2">
         <v>39</v>
       </c>
@@ -7284,13 +7255,13 @@
         <v>39</v>
       </c>
       <c r="W56" t="s" s="2">
-        <v>39</v>
+        <v>264</v>
       </c>
       <c r="X56" t="s" s="2">
-        <v>39</v>
+        <v>337</v>
       </c>
       <c r="Y56" t="s" s="2">
-        <v>39</v>
+        <v>338</v>
       </c>
       <c r="Z56" t="s" s="2">
         <v>39</v>
@@ -7308,13 +7279,13 @@
         <v>39</v>
       </c>
       <c r="AE56" t="s" s="2">
-        <v>328</v>
+        <v>332</v>
       </c>
       <c r="AF56" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AG56" t="s" s="2">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="AH56" t="s" s="2">
         <v>39</v>
@@ -7323,18 +7294,18 @@
         <v>59</v>
       </c>
       <c r="AJ56" t="s" s="2">
-        <v>331</v>
+        <v>39</v>
       </c>
       <c r="AK56" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AL56" t="s" s="2">
-        <v>332</v>
+        <v>339</v>
       </c>
     </row>
-    <row r="57" hidden="true">
+    <row r="57">
       <c r="A57" t="s" s="2">
-        <v>333</v>
+        <v>340</v>
       </c>
       <c r="B57" s="2"/>
       <c r="C57" t="s" s="2">
@@ -7345,10 +7316,10 @@
         <v>40</v>
       </c>
       <c r="F57" t="s" s="2">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="G57" t="s" s="2">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="H57" t="s" s="2">
         <v>39</v>
@@ -7357,13 +7328,13 @@
         <v>39</v>
       </c>
       <c r="J57" t="s" s="2">
-        <v>334</v>
+        <v>341</v>
       </c>
       <c r="K57" t="s" s="2">
-        <v>335</v>
+        <v>342</v>
       </c>
       <c r="L57" t="s" s="2">
-        <v>336</v>
+        <v>343</v>
       </c>
       <c r="M57" s="2"/>
       <c r="N57" s="2"/>
@@ -7390,13 +7361,13 @@
         <v>39</v>
       </c>
       <c r="W57" t="s" s="2">
-        <v>174</v>
+        <v>39</v>
       </c>
       <c r="X57" t="s" s="2">
-        <v>337</v>
+        <v>39</v>
       </c>
       <c r="Y57" t="s" s="2">
-        <v>338</v>
+        <v>39</v>
       </c>
       <c r="Z57" t="s" s="2">
         <v>39</v>
@@ -7414,13 +7385,13 @@
         <v>39</v>
       </c>
       <c r="AE57" t="s" s="2">
-        <v>333</v>
+        <v>340</v>
       </c>
       <c r="AF57" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AG57" t="s" s="2">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="AH57" t="s" s="2">
         <v>39</v>
@@ -7429,233 +7400,17 @@
         <v>59</v>
       </c>
       <c r="AJ57" t="s" s="2">
-        <v>339</v>
+        <v>344</v>
       </c>
       <c r="AK57" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AL57" t="s" s="2">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="58" hidden="true">
-      <c r="A58" t="s" s="2">
-        <v>341</v>
-      </c>
-      <c r="B58" s="2"/>
-      <c r="C58" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="D58" s="2"/>
-      <c r="E58" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="F58" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="G58" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="H58" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="I58" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="J58" t="s" s="2">
-        <v>170</v>
-      </c>
-      <c r="K58" t="s" s="2">
-        <v>342</v>
-      </c>
-      <c r="L58" t="s" s="2">
-        <v>343</v>
-      </c>
-      <c r="M58" t="s" s="2">
-        <v>344</v>
-      </c>
-      <c r="N58" t="s" s="2">
         <v>345</v>
-      </c>
-      <c r="O58" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="P58" s="2"/>
-      <c r="Q58" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="R58" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="S58" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="T58" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="U58" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="V58" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="W58" t="s" s="2">
-        <v>273</v>
-      </c>
-      <c r="X58" t="s" s="2">
-        <v>346</v>
-      </c>
-      <c r="Y58" t="s" s="2">
-        <v>347</v>
-      </c>
-      <c r="Z58" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AA58" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AB58" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AC58" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AD58" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AE58" t="s" s="2">
-        <v>341</v>
-      </c>
-      <c r="AF58" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AG58" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AH58" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AI58" t="s" s="2">
-        <v>59</v>
-      </c>
-      <c r="AJ58" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AK58" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AL58" t="s" s="2">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="s" s="2">
-        <v>349</v>
-      </c>
-      <c r="B59" s="2"/>
-      <c r="C59" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="D59" s="2"/>
-      <c r="E59" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="F59" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="G59" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="H59" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="I59" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="J59" t="s" s="2">
-        <v>350</v>
-      </c>
-      <c r="K59" t="s" s="2">
-        <v>351</v>
-      </c>
-      <c r="L59" t="s" s="2">
-        <v>352</v>
-      </c>
-      <c r="M59" s="2"/>
-      <c r="N59" s="2"/>
-      <c r="O59" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="P59" s="2"/>
-      <c r="Q59" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="R59" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="S59" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="T59" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="U59" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="V59" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="W59" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="X59" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="Y59" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="Z59" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AA59" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AB59" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AC59" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AD59" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AE59" t="s" s="2">
-        <v>349</v>
-      </c>
-      <c r="AF59" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AG59" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AH59" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AI59" t="s" s="2">
-        <v>59</v>
-      </c>
-      <c r="AJ59" t="s" s="2">
-        <v>353</v>
-      </c>
-      <c r="AK59" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AL59" t="s" s="2">
-        <v>354</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AL59">
+  <autoFilter ref="A1:AL57">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -7665,7 +7420,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI58">
+  <conditionalFormatting sqref="A2:AI56">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>